<commit_message>
CashFlow Updated (and changed price formula)
</commit_message>
<xml_diff>
--- a/CashFlow.xlsx
+++ b/CashFlow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Rafael Soares\Documents\GitHub\GPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Catarina\Documents\FACULDADE\MEIC\GPI\ProjetoAtual\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8834DF-9874-40DC-9D61-354B076270DC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8472441-8227-4F1A-B645-D2EA44126352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{3E8206BC-8C07-4571-9047-564953AB6915}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{3E8206BC-8C07-4571-9047-564953AB6915}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Resource Name</t>
   </si>
   <si>
-    <t>Cost</t>
-  </si>
-  <si>
     <t>Project Manager</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>Cash Flow</t>
   </si>
   <si>
-    <t>PHR Framework Cost</t>
-  </si>
-  <si>
     <t>PHR Framework License</t>
   </si>
   <si>
@@ -117,7 +111,10 @@
     <t>Finished Warranty Time</t>
   </si>
   <si>
-    <t xml:space="preserve">HR Cost </t>
+    <t>HR Costs</t>
+  </si>
+  <si>
+    <t>PHR Framework License Price</t>
   </si>
 </sst>
 </file>
@@ -127,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +145,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri "/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -158,18 +176,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDFE3E8"/>
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -203,32 +221,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB1BBCC"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFB1BBCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB1BBCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -247,7 +320,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -545,288 +618,305 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FDA0994-5B2E-4A19-B4D3-B7EC51AAD736}">
   <dimension ref="E6:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="D11" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="13.5234375" customWidth="1"/>
-    <col min="6" max="6" width="18.3125" customWidth="1"/>
-    <col min="7" max="7" width="10.05078125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.9453125" customWidth="1"/>
-    <col min="9" max="10" width="10.62890625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.20703125" customWidth="1"/>
-    <col min="12" max="13" width="10.05078125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.83984375" customWidth="1"/>
-    <col min="15" max="15" width="10.05078125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="9.05078125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F6" s="2" t="s">
+    <row r="6" spans="5:15">
+      <c r="F6" s="8"/>
+      <c r="G6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="5:15">
+      <c r="F7" s="9"/>
+      <c r="G7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F7" s="3" t="s">
+      <c r="H7" s="12">
+        <v>3850</v>
+      </c>
+      <c r="I7" s="12">
+        <v>1750</v>
+      </c>
+      <c r="J7" s="12">
+        <v>1400</v>
+      </c>
+      <c r="K7" s="12">
+        <v>2100</v>
+      </c>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="12">
+        <v>350</v>
+      </c>
+      <c r="O7" s="10"/>
+    </row>
+    <row r="8" spans="5:15" ht="30">
+      <c r="F8" s="9"/>
+      <c r="G8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="4">
-        <v>9450</v>
-      </c>
-      <c r="H7" s="1">
-        <v>3850</v>
-      </c>
-      <c r="I7" s="1">
-        <v>1750</v>
-      </c>
-      <c r="J7" s="1">
-        <v>1400</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="H8" s="12">
+        <v>3000</v>
+      </c>
+      <c r="I8" s="12">
+        <v>5500</v>
+      </c>
+      <c r="J8" s="12">
+        <v>4000</v>
+      </c>
+      <c r="K8" s="12">
+        <v>5000</v>
+      </c>
+      <c r="L8" s="12">
+        <v>525</v>
+      </c>
+      <c r="M8" s="12">
+        <v>500</v>
+      </c>
+      <c r="N8" s="12">
+        <v>475</v>
+      </c>
+      <c r="O8" s="10"/>
+    </row>
+    <row r="9" spans="5:15">
+      <c r="F9" s="9"/>
+      <c r="G9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="12">
+        <v>750</v>
+      </c>
+      <c r="I9" s="12">
+        <v>4750</v>
+      </c>
+      <c r="J9" s="12">
+        <v>4500</v>
+      </c>
+      <c r="K9" s="12">
+        <v>2500</v>
+      </c>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+    </row>
+    <row r="10" spans="5:15">
+      <c r="F10" s="9"/>
+      <c r="G10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="12">
+        <v>1650</v>
+      </c>
+      <c r="J10" s="12">
         <v>2100</v>
       </c>
-      <c r="N7" s="1">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="8" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="4">
-        <v>18750</v>
-      </c>
-      <c r="H8" s="1">
-        <v>3000</v>
-      </c>
-      <c r="I8" s="1">
-        <v>5500</v>
-      </c>
-      <c r="J8" s="1">
-        <v>4000</v>
-      </c>
-      <c r="K8" s="1">
-        <v>5000</v>
-      </c>
-      <c r="L8" s="1">
-        <v>525</v>
-      </c>
-      <c r="M8" s="1">
-        <v>500</v>
-      </c>
-      <c r="N8" s="1">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="9" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="4">
-        <v>12500</v>
-      </c>
-      <c r="H9" s="1">
-        <v>750</v>
-      </c>
-      <c r="I9" s="1">
-        <v>4750</v>
-      </c>
-      <c r="J9" s="1">
-        <v>4500</v>
-      </c>
-      <c r="K9" s="1">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="10" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F10" s="3" t="s">
+      <c r="K10" s="12">
+        <v>2700</v>
+      </c>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="10"/>
+    </row>
+    <row r="11" spans="5:15">
+      <c r="F11" s="9"/>
+      <c r="G11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="4">
-        <v>6450</v>
-      </c>
-      <c r="I10" s="1">
-        <v>1650</v>
-      </c>
-      <c r="J10" s="1">
-        <v>2100</v>
-      </c>
-      <c r="K10" s="1">
+      <c r="H11" s="10"/>
+      <c r="I11" s="12">
+        <v>1800</v>
+      </c>
+      <c r="J11" s="12">
+        <v>1500</v>
+      </c>
+      <c r="K11" s="12">
+        <v>3150</v>
+      </c>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+    </row>
+    <row r="12" spans="5:15">
+      <c r="F12" s="9"/>
+      <c r="G12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="12">
+        <v>2550</v>
+      </c>
+      <c r="J12" s="12">
         <v>2700</v>
       </c>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="4">
-        <v>6450</v>
-      </c>
-      <c r="I11" s="1">
-        <v>1800</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="K12" s="12">
         <v>1500</v>
       </c>
-      <c r="K11" s="1">
-        <v>3150</v>
-      </c>
-    </row>
-    <row r="12" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F12" s="3" t="s">
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+    </row>
+    <row r="13" spans="5:15">
+      <c r="F13" s="9"/>
+      <c r="G13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="4">
-        <v>6750</v>
-      </c>
-      <c r="I12" s="1">
+      <c r="H13" s="10"/>
+      <c r="I13" s="12">
         <v>2550</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J13" s="12">
         <v>2700</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K13" s="12">
         <v>1500</v>
       </c>
-    </row>
-    <row r="13" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F13" s="3" t="s">
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+    </row>
+    <row r="14" spans="5:15">
+      <c r="F14" s="9"/>
+      <c r="G14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="4">
-        <v>6750</v>
-      </c>
-      <c r="I13" s="1">
-        <v>2550</v>
-      </c>
-      <c r="J13" s="1">
-        <v>2700</v>
-      </c>
-      <c r="K13" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="14" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="4">
-        <v>4200</v>
-      </c>
-      <c r="I14" s="1">
+      <c r="H14" s="10"/>
+      <c r="I14" s="12">
         <v>1300</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="12">
         <v>1200</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="12">
         <v>1700</v>
       </c>
-    </row>
-    <row r="15" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="E15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="1">
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+    </row>
+    <row r="15" spans="5:15">
+      <c r="E15" s="4"/>
+      <c r="G15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="12">
         <f>SUM(H7:H14)</f>
         <v>7600</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="12">
         <f t="shared" ref="I15:N15" si="0">SUM(I7:I14)</f>
         <v>21850</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="12">
         <f t="shared" si="0"/>
         <v>20100</v>
       </c>
-      <c r="K15" s="1">
+      <c r="K15" s="12">
         <f t="shared" si="0"/>
         <v>20150</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L15" s="12">
         <f t="shared" si="0"/>
         <v>525</v>
       </c>
-      <c r="M15" s="1">
+      <c r="M15" s="12">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="12">
         <f t="shared" si="0"/>
         <v>825</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="12">
         <f>SUM(H15:N15)</f>
         <v>71550</v>
       </c>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="E18" t="s">
+    <row r="18" spans="5:15">
+      <c r="F18" s="5"/>
+      <c r="G18" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="1">
+        <f>(O15+O21)*I19 + (O15+O21)</f>
+        <v>139437.5</v>
+      </c>
+    </row>
+    <row r="19" spans="5:15">
+      <c r="G19" s="6"/>
+      <c r="H19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18">
-        <v>140000</v>
-      </c>
-    </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="8">
-        <f>(G18-O15-O21)/(O15+O21)</f>
-        <v>0.25504258180188255</v>
-      </c>
-    </row>
-    <row r="21" spans="5:15" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="E21" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
+      <c r="I19" s="18">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="21" spans="5:15" ht="30">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="17" t="s">
+        <v>21</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="K21" s="1"/>
       <c r="O21" s="1">
         <v>40000</v>
       </c>
     </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="E22" t="s">
-        <v>22</v>
-      </c>
-      <c r="G22" s="4"/>
+    <row r="22" spans="5:15">
+      <c r="G22" s="16" t="s">
+        <v>27</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="K22" s="1"/>
       <c r="O22" s="1">
@@ -834,229 +924,195 @@
         <v>48000</v>
       </c>
     </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="E27" t="s">
+    <row r="27" spans="5:15">
+      <c r="G27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H27" t="s">
-        <v>26</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="N27" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="E28" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="H28" s="7">
+    </row>
+    <row r="28" spans="5:15">
+      <c r="F28" s="2"/>
+      <c r="G28" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="19">
         <v>0.2</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="19">
         <v>0</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="19">
         <v>0</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K28" s="19">
         <v>0.5</v>
       </c>
-      <c r="L28" s="7">
+      <c r="L28" s="19">
         <v>0</v>
       </c>
-      <c r="M28" s="7">
+      <c r="M28" s="19">
         <v>0</v>
       </c>
-      <c r="N28" s="7">
+      <c r="N28" s="19">
         <v>0.3</v>
       </c>
     </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F29" s="3"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="1">
-        <f>$G18*H28</f>
-        <v>28000</v>
-      </c>
-      <c r="I29" s="1">
-        <f>$G18*I28</f>
+    <row r="29" spans="5:15">
+      <c r="F29" s="2"/>
+      <c r="H29" s="12">
+        <f>$I18*H28</f>
+        <v>27887.5</v>
+      </c>
+      <c r="I29" s="12">
+        <f>$I18*I28</f>
         <v>0</v>
       </c>
-      <c r="J29" s="1">
-        <f>$G18*J28</f>
+      <c r="J29" s="12">
+        <f>$I18*J28</f>
         <v>0</v>
       </c>
-      <c r="K29" s="1">
-        <f>$G18*K28</f>
-        <v>70000</v>
-      </c>
-      <c r="L29" s="1">
-        <f>$G18*L28</f>
+      <c r="K29" s="12">
+        <f>$I18*K28</f>
+        <v>69718.75</v>
+      </c>
+      <c r="L29" s="12">
+        <f>$I18*L28</f>
         <v>0</v>
       </c>
-      <c r="M29" s="1">
-        <f>$G18*M28</f>
+      <c r="M29" s="12">
+        <f>$I18*M28</f>
         <v>0</v>
       </c>
-      <c r="N29" s="1">
-        <f>$G18*N28</f>
-        <v>42000</v>
-      </c>
-    </row>
-    <row r="30" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="F30" s="3"/>
-      <c r="G30" s="4"/>
+      <c r="N29" s="12">
+        <f>$I18*N28</f>
+        <v>41831.25</v>
+      </c>
+    </row>
+    <row r="30" spans="5:15">
+      <c r="F30" s="2"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="5:15" x14ac:dyDescent="0.55000000000000004">
-      <c r="E31" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" s="1">
+    <row r="31" spans="5:15">
+      <c r="G31" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="15">
         <f>H29-H15</f>
-        <v>20400</v>
-      </c>
-      <c r="I31" s="1">
-        <f>H31+I29-I15</f>
-        <v>-1450</v>
-      </c>
-      <c r="J31" s="1">
-        <f>I31+J29-J15</f>
-        <v>-21550</v>
-      </c>
-      <c r="K31" s="1">
-        <f>J31+K29-K15</f>
-        <v>28300</v>
-      </c>
-      <c r="L31" s="1">
-        <f>K31+L29-L15</f>
-        <v>27775</v>
-      </c>
-      <c r="M31" s="1">
-        <f>L31+M29-M15</f>
-        <v>27275</v>
-      </c>
-      <c r="N31" s="1">
-        <f>M31+N29-N15</f>
-        <v>68450</v>
-      </c>
-    </row>
-    <row r="39" spans="7:12" ht="27" x14ac:dyDescent="0.55000000000000004">
-      <c r="G39" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="7:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G40" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H40" s="4">
-        <v>9450</v>
-      </c>
-    </row>
-    <row r="41" spans="7:12" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="G41" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H41" s="4">
-        <v>19000</v>
-      </c>
-    </row>
-    <row r="42" spans="7:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H42" s="4">
-        <v>12500</v>
-      </c>
-    </row>
-    <row r="43" spans="7:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G43" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H43" s="4">
-        <v>6450</v>
-      </c>
-    </row>
-    <row r="44" spans="7:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G44" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H44" s="4">
-        <v>6450</v>
-      </c>
-    </row>
-    <row r="45" spans="7:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G45" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" s="4">
-        <v>6750</v>
-      </c>
-    </row>
-    <row r="46" spans="7:12" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="G46" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H46" s="4">
-        <v>6750</v>
-      </c>
-    </row>
-    <row r="47" spans="7:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="G47" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H47" s="4">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="48" spans="7:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="G48" s="3"/>
-      <c r="H48" s="4"/>
+        <v>20287.5</v>
+      </c>
+      <c r="I31" s="15">
+        <f t="shared" ref="I31:N31" si="1">H31+I29-I15</f>
+        <v>-1562.5</v>
+      </c>
+      <c r="J31" s="15">
+        <f t="shared" si="1"/>
+        <v>-21662.5</v>
+      </c>
+      <c r="K31" s="15">
+        <f t="shared" si="1"/>
+        <v>27906.25</v>
+      </c>
+      <c r="L31" s="15">
+        <f t="shared" si="1"/>
+        <v>27381.25</v>
+      </c>
+      <c r="M31" s="15">
+        <f t="shared" si="1"/>
+        <v>26881.25</v>
+      </c>
+      <c r="N31" s="15">
+        <f t="shared" si="1"/>
+        <v>67887.5</v>
+      </c>
+    </row>
+    <row r="39" spans="7:12">
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+    </row>
+    <row r="40" spans="7:12">
+      <c r="G40" s="2"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="7:12">
+      <c r="G41" s="2"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="7:12">
+      <c r="G42" s="2"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="7:12">
+      <c r="G43" s="2"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="7:12">
+      <c r="G44" s="2"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="7:12">
+      <c r="G45" s="2"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="7:12">
+      <c r="G46" s="2"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="7:12">
+      <c r="G47" s="2"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="7:12">
+      <c r="G48" s="2"/>
+      <c r="H48" s="3"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="54" spans="7:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="G54" s="3"/>
-      <c r="H54" s="4"/>
+    <row r="54" spans="7:12">
+      <c r="G54" s="2"/>
+      <c r="H54" s="3"/>
       <c r="I54" s="1"/>
       <c r="L54" s="1"/>
     </row>
-    <row r="55" spans="7:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="G55" s="3"/>
-      <c r="H55" s="4"/>
+    <row r="55" spans="7:12">
+      <c r="G55" s="2"/>
+      <c r="H55" s="3"/>
       <c r="I55" s="1"/>
       <c r="L55" s="1"/>
     </row>
-    <row r="56" spans="7:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="G56" s="3"/>
-      <c r="H56" s="4"/>
+    <row r="56" spans="7:12">
+      <c r="G56" s="2"/>
+      <c r="H56" s="3"/>
       <c r="I56" s="1"/>
       <c r="L56" s="1"/>
     </row>
-    <row r="57" spans="7:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="G57" s="3"/>
-      <c r="H57" s="4"/>
+    <row r="57" spans="7:12">
+      <c r="G57" s="2"/>
+      <c r="H57" s="3"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
     </row>
-    <row r="58" spans="7:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="G58" s="3"/>
-      <c r="H58" s="4"/>
+    <row r="58" spans="7:12">
+      <c r="G58" s="2"/>
+      <c r="H58" s="3"/>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>

</xml_diff>

<commit_message>
All files final update
</commit_message>
<xml_diff>
--- a/CashFlow.xlsx
+++ b/CashFlow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Catarina\Documents\FACULDADE\MEIC\GPI\ProjetoAtual\GPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Rafael Soares\Documents\GitHub\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9AE34F4-5558-4F18-88ED-BBA307EF78D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A614C95E-40D5-4E21-81DB-F3155CE69C6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{3E8206BC-8C07-4571-9047-564953AB6915}"/>
+    <workbookView xWindow="1770" yWindow="1770" windowWidth="17280" windowHeight="8994" xr2:uid="{3E8206BC-8C07-4571-9047-564953AB6915}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -325,7 +325,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -623,22 +623,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FDA0994-5B2E-4A19-B4D3-B7EC51AAD736}">
   <dimension ref="E6:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.578125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.83984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.15625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.41796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.41796875" bestFit="1" customWidth="1"/>
     <col min="17" max="20" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -696,7 +696,7 @@
       </c>
       <c r="O7" s="20"/>
     </row>
-    <row r="8" spans="6:15" ht="30">
+    <row r="8" spans="6:15">
       <c r="F8" s="9"/>
       <c r="G8" s="11" t="s">
         <v>2</v>
@@ -708,19 +708,19 @@
         <v>5500</v>
       </c>
       <c r="J8" s="19">
-        <v>4000</v>
+        <v>4250</v>
       </c>
       <c r="K8" s="19">
-        <v>5000</v>
+        <v>5125</v>
       </c>
       <c r="L8" s="19">
-        <v>525</v>
+        <v>625</v>
       </c>
       <c r="M8" s="19">
         <v>500</v>
       </c>
       <c r="N8" s="19">
-        <v>475</v>
+        <v>500</v>
       </c>
       <c r="O8" s="20"/>
     </row>
@@ -756,12 +756,14 @@
         <v>1650</v>
       </c>
       <c r="J10" s="19">
-        <v>2100</v>
+        <v>2250</v>
       </c>
       <c r="K10" s="19">
         <v>2700</v>
       </c>
-      <c r="L10" s="20"/>
+      <c r="L10" s="19">
+        <v>150</v>
+      </c>
       <c r="M10" s="20"/>
       <c r="N10" s="19"/>
       <c r="O10" s="20"/>
@@ -776,12 +778,14 @@
         <v>1800</v>
       </c>
       <c r="J11" s="19">
-        <v>1500</v>
+        <v>1800</v>
       </c>
       <c r="K11" s="19">
-        <v>3150</v>
-      </c>
-      <c r="L11" s="20"/>
+        <v>3000</v>
+      </c>
+      <c r="L11" s="19">
+        <v>150</v>
+      </c>
       <c r="M11" s="20"/>
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
@@ -836,17 +840,19 @@
         <v>1300</v>
       </c>
       <c r="J14" s="19">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="K14" s="19">
-        <v>1700</v>
-      </c>
-      <c r="L14" s="20"/>
+        <v>1600</v>
+      </c>
+      <c r="L14" s="19">
+        <v>100</v>
+      </c>
       <c r="M14" s="20"/>
       <c r="N14" s="20"/>
       <c r="O14" s="20"/>
     </row>
-    <row r="15" spans="6:15" ht="30">
+    <row r="15" spans="6:15">
       <c r="F15" s="5"/>
       <c r="G15" s="11" t="s">
         <v>21</v>
@@ -893,15 +899,15 @@
       </c>
       <c r="J17" s="19">
         <f>SUM(J7:J15)</f>
-        <v>60100</v>
+        <v>61000</v>
       </c>
       <c r="K17" s="19">
         <f>SUM(K7:K14)</f>
-        <v>20150</v>
+        <v>20025</v>
       </c>
       <c r="L17" s="19">
         <f>SUM(L7:L14)</f>
-        <v>525</v>
+        <v>1025</v>
       </c>
       <c r="M17" s="19">
         <f>SUM(M7:M14)</f>
@@ -909,11 +915,11 @@
       </c>
       <c r="N17" s="19">
         <f>SUM(N7:N14)</f>
-        <v>825</v>
+        <v>850</v>
       </c>
       <c r="O17" s="19">
         <f>SUM(H17:N17)</f>
-        <v>111550</v>
+        <v>112850</v>
       </c>
     </row>
     <row r="18" spans="5:15">
@@ -929,7 +935,7 @@
       </c>
       <c r="I20" s="1">
         <f>(O17)*I21 + (O17)</f>
-        <v>145015</v>
+        <v>146705</v>
       </c>
     </row>
     <row r="21" spans="5:15">
@@ -1004,7 +1010,7 @@
       <c r="F31" s="2"/>
       <c r="H31" s="12">
         <f t="shared" ref="H31:N31" si="0">$I20*H30</f>
-        <v>29003</v>
+        <v>29341</v>
       </c>
       <c r="I31" s="12">
         <f t="shared" si="0"/>
@@ -1016,7 +1022,7 @@
       </c>
       <c r="K31" s="12">
         <f t="shared" si="0"/>
-        <v>72507.5</v>
+        <v>73352.5</v>
       </c>
       <c r="L31" s="12">
         <f t="shared" si="0"/>
@@ -1028,7 +1034,7 @@
       </c>
       <c r="N31" s="12">
         <f t="shared" si="0"/>
-        <v>43504.5</v>
+        <v>44011.5</v>
       </c>
     </row>
     <row r="32" spans="5:15">
@@ -1044,31 +1050,31 @@
       </c>
       <c r="H33" s="12">
         <f>H31-H17</f>
-        <v>21403</v>
+        <v>21741</v>
       </c>
       <c r="I33" s="12">
         <f t="shared" ref="I33:N33" si="1">H33+I31-I17</f>
-        <v>-447</v>
+        <v>-109</v>
       </c>
       <c r="J33" s="12">
         <f t="shared" si="1"/>
-        <v>-60547</v>
+        <v>-61109</v>
       </c>
       <c r="K33" s="12">
         <f t="shared" si="1"/>
-        <v>-8189.5</v>
+        <v>-7781.5</v>
       </c>
       <c r="L33" s="12">
         <f t="shared" si="1"/>
-        <v>-8714.5</v>
+        <v>-8806.5</v>
       </c>
       <c r="M33" s="12">
         <f t="shared" si="1"/>
-        <v>-9214.5</v>
+        <v>-9306.5</v>
       </c>
       <c r="N33" s="12">
         <f t="shared" si="1"/>
-        <v>33465</v>
+        <v>33855</v>
       </c>
     </row>
     <row r="41" spans="7:14">

</xml_diff>

<commit_message>
Final update on cash flow
</commit_message>
<xml_diff>
--- a/CashFlow.xlsx
+++ b/CashFlow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Rafael Soares\Documents\GitHub\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48943FC-A189-4E63-9113-44F7693E388B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C30FD4-3CBA-445A-8A78-2842A7ED4611}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{3E8206BC-8C07-4571-9047-564953AB6915}"/>
   </bookViews>
@@ -121,8 +121,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -297,7 +298,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -307,6 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,7 +625,7 @@
   <dimension ref="E6:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -677,247 +678,247 @@
       <c r="G7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="18">
         <v>3850</v>
       </c>
-      <c r="I7" s="19">
+      <c r="I7" s="18">
         <v>1750</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="18">
         <v>1400</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="18">
         <v>2100</v>
       </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="19">
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="18">
         <v>350</v>
       </c>
-      <c r="O7" s="20"/>
+      <c r="O7" s="19"/>
     </row>
     <row r="8" spans="6:15">
       <c r="F8" s="9"/>
       <c r="G8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="18">
         <v>3000</v>
       </c>
-      <c r="I8" s="19">
+      <c r="I8" s="18">
         <v>5500</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="18">
         <v>4250</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="18">
         <v>5125</v>
       </c>
-      <c r="L8" s="19">
+      <c r="L8" s="18">
         <v>625</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="18">
         <v>500</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="18">
         <v>500</v>
       </c>
-      <c r="O8" s="20"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="9" spans="6:15">
       <c r="F9" s="9"/>
       <c r="G9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="19">
+      <c r="H9" s="18">
         <v>750</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="18">
         <v>4750</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="18">
         <v>4500</v>
       </c>
-      <c r="K9" s="19">
+      <c r="K9" s="18">
         <v>2500</v>
       </c>
-      <c r="L9" s="20"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="20"/>
-      <c r="O9" s="20"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
     </row>
     <row r="10" spans="6:15">
       <c r="F10" s="9"/>
       <c r="G10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="19">
+      <c r="H10" s="19"/>
+      <c r="I10" s="18">
         <v>1650</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="18">
         <v>2250</v>
       </c>
-      <c r="K10" s="19">
+      <c r="K10" s="18">
         <v>2700</v>
       </c>
-      <c r="L10" s="19">
+      <c r="L10" s="18">
         <v>150</v>
       </c>
-      <c r="M10" s="20"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="20"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="19"/>
     </row>
     <row r="11" spans="6:15">
       <c r="F11" s="9"/>
       <c r="G11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="19">
+      <c r="H11" s="19"/>
+      <c r="I11" s="18">
         <v>1800</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="18">
         <v>1800</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="18">
         <v>3000</v>
       </c>
-      <c r="L11" s="19">
+      <c r="L11" s="18">
         <v>150</v>
       </c>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
-      <c r="O11" s="20"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
     </row>
     <row r="12" spans="6:15">
       <c r="F12" s="9"/>
       <c r="G12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="19">
+      <c r="H12" s="19"/>
+      <c r="I12" s="18">
         <v>2550</v>
       </c>
-      <c r="J12" s="19">
+      <c r="J12" s="18">
         <v>2700</v>
       </c>
-      <c r="K12" s="19">
+      <c r="K12" s="18">
         <v>1500</v>
       </c>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
-      <c r="O12" s="20"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
     </row>
     <row r="13" spans="6:15">
       <c r="F13" s="9"/>
       <c r="G13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="19">
+      <c r="H13" s="19"/>
+      <c r="I13" s="18">
         <v>2550</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="18">
         <v>2700</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="18">
         <v>1500</v>
       </c>
-      <c r="L13" s="20"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
-      <c r="O13" s="20"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
     </row>
     <row r="14" spans="6:15">
       <c r="F14" s="9"/>
       <c r="G14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="19">
+      <c r="H14" s="19"/>
+      <c r="I14" s="18">
         <v>1300</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="18">
         <v>1400</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="18">
         <v>1600</v>
       </c>
-      <c r="L14" s="19">
+      <c r="L14" s="18">
         <v>100</v>
       </c>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
-      <c r="O14" s="20"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
     </row>
     <row r="15" spans="6:15">
       <c r="F15" s="5"/>
       <c r="G15" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19">
+      <c r="H15" s="19"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18">
         <v>40000</v>
       </c>
-      <c r="K15" s="19"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
     </row>
     <row r="16" spans="6:15">
       <c r="F16" s="5"/>
       <c r="G16" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19">
+      <c r="H16" s="19"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18">
         <v>200</v>
       </c>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
     </row>
     <row r="17" spans="5:15">
       <c r="E17" s="4"/>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="19">
+      <c r="H17" s="18">
         <f t="shared" ref="H17:I17" si="0">SUM(H7:H16)</f>
         <v>7600</v>
       </c>
-      <c r="I17" s="19">
+      <c r="I17" s="18">
         <f t="shared" si="0"/>
         <v>21850</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="18">
         <f>SUM(J7:J16)</f>
         <v>61000</v>
       </c>
-      <c r="K17" s="19">
+      <c r="K17" s="18">
         <f t="shared" ref="K17:N17" si="1">SUM(K7:K16)</f>
         <v>20225</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="18">
         <f t="shared" si="1"/>
         <v>1025</v>
       </c>
-      <c r="M17" s="19">
+      <c r="M17" s="18">
         <f t="shared" si="1"/>
         <v>500</v>
       </c>
-      <c r="N17" s="19">
+      <c r="N17" s="18">
         <f t="shared" si="1"/>
         <v>850</v>
       </c>
-      <c r="O17" s="19">
+      <c r="O17" s="18">
         <f>SUM(H17:N17)</f>
         <v>113050</v>
       </c>
@@ -934,8 +935,7 @@
         <v>16</v>
       </c>
       <c r="I20" s="1">
-        <f>(O17)*I21 + (O17)</f>
-        <v>146965</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="21" spans="5:15">
@@ -943,8 +943,9 @@
       <c r="H21" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="17">
-        <v>0.3</v>
+      <c r="I21" s="20">
+        <f>(I20-O17)/O17</f>
+        <v>0.32684652808491815</v>
       </c>
     </row>
     <row r="23" spans="5:15">
@@ -984,25 +985,25 @@
       <c r="G30" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="17">
         <v>0.2</v>
       </c>
-      <c r="I30" s="18">
+      <c r="I30" s="17">
         <v>0</v>
       </c>
-      <c r="J30" s="18">
+      <c r="J30" s="17">
         <v>0</v>
       </c>
-      <c r="K30" s="18">
+      <c r="K30" s="17">
         <v>0.5</v>
       </c>
-      <c r="L30" s="18">
+      <c r="L30" s="17">
         <v>0</v>
       </c>
-      <c r="M30" s="18">
+      <c r="M30" s="17">
         <v>0</v>
       </c>
-      <c r="N30" s="18">
+      <c r="N30" s="17">
         <v>0.3</v>
       </c>
     </row>
@@ -1010,7 +1011,7 @@
       <c r="F31" s="2"/>
       <c r="H31" s="12">
         <f t="shared" ref="H31:N31" si="2">$I20*H30</f>
-        <v>29393</v>
+        <v>30000</v>
       </c>
       <c r="I31" s="12">
         <f t="shared" si="2"/>
@@ -1022,7 +1023,7 @@
       </c>
       <c r="K31" s="12">
         <f t="shared" si="2"/>
-        <v>73482.5</v>
+        <v>75000</v>
       </c>
       <c r="L31" s="12">
         <f t="shared" si="2"/>
@@ -1034,7 +1035,7 @@
       </c>
       <c r="N31" s="12">
         <f t="shared" si="2"/>
-        <v>44089.5</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="32" spans="5:15">
@@ -1050,31 +1051,31 @@
       </c>
       <c r="H33" s="12">
         <f>H31-H17</f>
-        <v>21793</v>
+        <v>22400</v>
       </c>
       <c r="I33" s="12">
         <f t="shared" ref="I33:N33" si="3">H33+I31-I17</f>
-        <v>-57</v>
+        <v>550</v>
       </c>
       <c r="J33" s="12">
         <f t="shared" si="3"/>
-        <v>-61057</v>
+        <v>-60450</v>
       </c>
       <c r="K33" s="12">
         <f t="shared" si="3"/>
-        <v>-7799.5</v>
+        <v>-5675</v>
       </c>
       <c r="L33" s="12">
         <f t="shared" si="3"/>
-        <v>-8824.5</v>
+        <v>-6700</v>
       </c>
       <c r="M33" s="12">
         <f t="shared" si="3"/>
-        <v>-9324.5</v>
+        <v>-7200</v>
       </c>
       <c r="N33" s="12">
         <f t="shared" si="3"/>
-        <v>33915</v>
+        <v>36950</v>
       </c>
     </row>
     <row r="41" spans="7:14">

</xml_diff>

<commit_message>
Added changes and reports
</commit_message>
<xml_diff>
--- a/CashFlow.xlsx
+++ b/CashFlow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Rafael Soares\Documents\GitHub\GPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572F9D3B-77E3-4EA5-AA42-9D2DDE2D4F3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3EA841-C122-4079-8999-350E20686DB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{3E8206BC-8C07-4571-9047-564953AB6915}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Resource Name</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>M8</t>
+  </si>
+  <si>
+    <t>M9</t>
   </si>
 </sst>
 </file>
@@ -325,8 +328,8 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FDA0994-5B2E-4A19-B4D3-B7EC51AAD736}">
-  <dimension ref="E6:P58"/>
+  <dimension ref="E6:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F12" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -660,11 +663,11 @@
     <col min="12" max="13" width="11.15625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.41796875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.41796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.05078125" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.05078125" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="6:16">
+    <row r="6" spans="6:17">
       <c r="F6" s="8"/>
       <c r="G6" s="14" t="s">
         <v>0</v>
@@ -694,18 +697,21 @@
         <v>28</v>
       </c>
       <c r="P6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" s="22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="6:16">
+    <row r="7" spans="6:17">
       <c r="F7" s="9"/>
       <c r="G7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="1">
         <v>3500</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="1">
         <v>1750</v>
       </c>
       <c r="J7" s="1">
@@ -714,52 +720,55 @@
       <c r="K7" s="1">
         <v>1050</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>1050</v>
       </c>
-      <c r="O7" s="1">
+      <c r="P7" s="1">
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="6:16">
+    <row r="8" spans="6:17">
       <c r="F8" s="9"/>
       <c r="G8" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="3">
         <v>2500</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="1">
         <v>5250</v>
       </c>
       <c r="J8" s="1">
-        <v>4250</v>
+        <v>5000</v>
       </c>
       <c r="K8" s="1">
-        <v>2750</v>
+        <v>3750</v>
       </c>
       <c r="L8" s="1">
-        <v>4750</v>
+        <v>4500</v>
       </c>
       <c r="M8" s="1">
-        <v>500</v>
+        <v>1350</v>
       </c>
       <c r="N8" s="1">
         <v>525</v>
       </c>
       <c r="O8" s="1">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="9" spans="6:16">
+        <v>575</v>
+      </c>
+      <c r="P8" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="6:17">
       <c r="F9" s="9"/>
       <c r="G9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="3">
         <v>500</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="1">
         <v>3000</v>
       </c>
       <c r="J9" s="1">
@@ -769,50 +778,63 @@
         <v>4000</v>
       </c>
       <c r="L9" s="1">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="10" spans="6:16">
+        <v>2250</v>
+      </c>
+      <c r="M9" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="6:17">
       <c r="F10" s="9"/>
       <c r="G10" s="11" t="s">
         <v>4</v>
       </c>
+      <c r="H10" s="3"/>
       <c r="I10" s="1">
         <v>1800</v>
       </c>
       <c r="J10" s="1">
-        <v>1950</v>
+        <v>2400</v>
       </c>
       <c r="K10" s="1">
-        <v>1200</v>
+        <v>1800</v>
       </c>
       <c r="L10" s="1">
-        <v>2550</v>
-      </c>
-    </row>
-    <row r="11" spans="6:16">
+        <v>2100</v>
+      </c>
+      <c r="M10" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="11" spans="6:17">
       <c r="F11" s="9"/>
       <c r="G11" s="11" t="s">
         <v>5</v>
       </c>
+      <c r="H11" s="3"/>
       <c r="I11" s="1">
         <v>1650</v>
       </c>
       <c r="J11" s="1">
-        <v>1950</v>
+        <v>2700</v>
       </c>
       <c r="K11" s="1">
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="L11" s="1">
-        <v>3150</v>
-      </c>
-    </row>
-    <row r="12" spans="6:16">
+        <v>2250</v>
+      </c>
+      <c r="M11" s="1">
+        <v>900</v>
+      </c>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="6:17">
       <c r="F12" s="9"/>
       <c r="G12" s="11" t="s">
         <v>6</v>
       </c>
+      <c r="H12" s="3"/>
       <c r="I12" s="1">
         <v>1350</v>
       </c>
@@ -823,14 +845,19 @@
         <v>2400</v>
       </c>
       <c r="L12" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="13" spans="6:16">
+        <v>1350</v>
+      </c>
+      <c r="M12" s="1">
+        <v>150</v>
+      </c>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="6:17">
       <c r="F13" s="9"/>
       <c r="G13" s="11" t="s">
         <v>7</v>
       </c>
+      <c r="H13" s="3"/>
       <c r="I13" s="1">
         <v>1350</v>
       </c>
@@ -841,28 +868,36 @@
         <v>2400</v>
       </c>
       <c r="L13" s="1">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="14" spans="6:16">
+        <v>1350</v>
+      </c>
+      <c r="M13" s="1">
+        <v>150</v>
+      </c>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="6:17">
       <c r="F14" s="9"/>
       <c r="G14" s="11" t="s">
         <v>8</v>
       </c>
+      <c r="H14" s="3"/>
       <c r="I14" s="1">
         <v>700</v>
       </c>
       <c r="J14" s="1">
-        <v>1500</v>
+        <v>1800</v>
       </c>
       <c r="K14" s="1">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="L14" s="1">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="15" spans="6:16">
+        <v>1100</v>
+      </c>
+      <c r="M14" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="15" spans="6:17">
       <c r="F15" s="5"/>
       <c r="G15" s="11" t="s">
         <v>21</v>
@@ -878,7 +913,7 @@
       <c r="N15" s="19"/>
       <c r="O15" s="19"/>
     </row>
-    <row r="16" spans="6:16">
+    <row r="16" spans="6:17">
       <c r="F16" s="5"/>
       <c r="G16" s="11" t="s">
         <v>27</v>
@@ -894,34 +929,34 @@
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
     </row>
-    <row r="17" spans="5:16">
+    <row r="17" spans="5:17">
       <c r="E17" s="4"/>
       <c r="G17" s="19" t="s">
         <v>26</v>
       </c>
       <c r="H17" s="18">
-        <f t="shared" ref="H17:P17" si="0">SUM(H7:H16)</f>
+        <f>SUM(H7:H16)</f>
         <v>6500</v>
       </c>
       <c r="I17" s="18">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I17:P17" si="0">SUM(I7:I16)</f>
         <v>16850</v>
       </c>
       <c r="J17" s="18">
         <f t="shared" si="0"/>
-        <v>62050</v>
+        <v>64300</v>
       </c>
       <c r="K17" s="18">
         <f t="shared" si="0"/>
-        <v>15250</v>
+        <v>18300</v>
       </c>
       <c r="L17" s="18">
         <f t="shared" si="0"/>
-        <v>18700</v>
+        <v>14900</v>
       </c>
       <c r="M17" s="18">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>5350</v>
       </c>
       <c r="N17" s="18">
         <f t="shared" si="0"/>
@@ -929,17 +964,21 @@
       </c>
       <c r="O17" s="18">
         <f t="shared" si="0"/>
-        <v>825</v>
-      </c>
-      <c r="P17" s="22">
-        <f>SUM(H17:O17)</f>
-        <v>121200</v>
-      </c>
-    </row>
-    <row r="18" spans="5:16">
+        <v>575</v>
+      </c>
+      <c r="P17" s="18">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>SUM(H17:P17)</f>
+        <v>127700</v>
+      </c>
+    </row>
+    <row r="18" spans="5:17">
       <c r="G18" s="16"/>
     </row>
-    <row r="20" spans="5:16">
+    <row r="20" spans="5:17">
       <c r="F20" s="5"/>
       <c r="G20" s="15" t="s">
         <v>17</v>
@@ -951,17 +990,17 @@
         <v>150000</v>
       </c>
     </row>
-    <row r="21" spans="5:16">
+    <row r="21" spans="5:17">
       <c r="G21" s="6"/>
       <c r="H21" s="6" t="s">
         <v>18</v>
       </c>
       <c r="I21" s="20">
-        <f>(I20-P17)/P17</f>
-        <v>0.23762376237623761</v>
-      </c>
-    </row>
-    <row r="23" spans="5:16">
+        <f>(I20-Q17)/Q17</f>
+        <v>0.17462803445575567</v>
+      </c>
+    </row>
+    <row r="23" spans="5:17">
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="16"/>
@@ -969,13 +1008,13 @@
       <c r="K23" s="1"/>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="5:16">
+    <row r="24" spans="5:17">
       <c r="G24" s="15"/>
       <c r="H24" s="1"/>
       <c r="K24" s="1"/>
       <c r="O24" s="1"/>
     </row>
-    <row r="29" spans="5:16">
+    <row r="29" spans="5:17">
       <c r="G29" s="15" t="s">
         <v>22</v>
       </c>
@@ -993,7 +1032,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="5:16">
+    <row r="30" spans="5:17">
       <c r="F30" s="2"/>
       <c r="G30" s="15" t="s">
         <v>19</v>
@@ -1023,7 +1062,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="31" spans="5:16">
+    <row r="31" spans="5:17">
       <c r="F31" s="2"/>
       <c r="H31" s="12">
         <f t="shared" ref="H31:N31" si="1">$I20*H30</f>
@@ -1058,14 +1097,14 @@
         <v>45000</v>
       </c>
     </row>
-    <row r="32" spans="5:16">
+    <row r="32" spans="5:17">
       <c r="F32" s="2"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="7:15">
+    <row r="33" spans="7:16">
       <c r="G33" s="15" t="s">
         <v>20</v>
       </c>
@@ -1074,97 +1113,87 @@
         <v>23500</v>
       </c>
       <c r="I33" s="12">
-        <f t="shared" ref="I33:N33" si="2">H33+I31-I17</f>
+        <f t="shared" ref="I33" si="2">H33+I31-I17</f>
         <v>6650</v>
       </c>
       <c r="J33" s="12">
         <f t="shared" ref="J33" si="3">I33+J31-J17</f>
-        <v>-55400</v>
+        <v>-57650</v>
       </c>
       <c r="K33" s="12">
         <f t="shared" ref="K33" si="4">J33+K31-K17</f>
-        <v>4350</v>
+        <v>-950</v>
       </c>
       <c r="L33" s="12">
         <f t="shared" ref="L33" si="5">K33+L31-L17</f>
-        <v>-14350</v>
+        <v>-15850</v>
       </c>
       <c r="M33" s="12">
         <f t="shared" ref="M33" si="6">L33+M31-M17</f>
-        <v>-14850</v>
+        <v>-21200</v>
       </c>
       <c r="N33" s="12">
         <f t="shared" ref="N33" si="7">M33+N31-N17</f>
-        <v>-15375</v>
+        <v>-21725</v>
       </c>
       <c r="O33" s="12">
         <f t="shared" ref="O33" si="8">N33+O31-O17</f>
-        <v>28800</v>
-      </c>
-    </row>
-    <row r="41" spans="7:15">
+        <v>22700</v>
+      </c>
+    </row>
+    <row r="37" spans="7:16">
+      <c r="H37" s="1"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="7:16">
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="7:16">
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="7:16">
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="7:16">
       <c r="G41" s="7"/>
-      <c r="H41" s="7"/>
-    </row>
-    <row r="42" spans="7:15">
+    </row>
+    <row r="42" spans="7:16">
       <c r="G42" s="21"/>
-      <c r="H42" s="3"/>
-      <c r="K42" s="1"/>
-    </row>
-    <row r="43" spans="7:15">
+    </row>
+    <row r="43" spans="7:16">
       <c r="G43" s="21"/>
-      <c r="H43" s="3"/>
-      <c r="K43" s="1"/>
-    </row>
-    <row r="44" spans="7:15">
+    </row>
+    <row r="44" spans="7:16">
       <c r="G44" s="21"/>
-      <c r="H44" s="3"/>
-      <c r="K44" s="1"/>
-    </row>
-    <row r="45" spans="7:15">
+    </row>
+    <row r="45" spans="7:16">
       <c r="G45" s="21"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="N45" s="1"/>
-    </row>
-    <row r="46" spans="7:15">
+    </row>
+    <row r="46" spans="7:16">
       <c r="G46" s="21"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="N46" s="1"/>
-    </row>
-    <row r="47" spans="7:15">
+    </row>
+    <row r="47" spans="7:16">
       <c r="G47" s="21"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-    </row>
-    <row r="48" spans="7:15">
+    </row>
+    <row r="48" spans="7:16">
       <c r="G48" s="21"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
     </row>
     <row r="49" spans="7:12">
       <c r="H49" s="1"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
     </row>
     <row r="50" spans="7:12">
       <c r="H50" s="1"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
     </row>
     <row r="51" spans="7:12">
       <c r="H51" s="1"/>

</xml_diff>